<commit_message>
-Added Sprint 4 Retro
</commit_message>
<xml_diff>
--- a/documents/Release 2 Plan.xlsx
+++ b/documents/Release 2 Plan.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franciscobarafani/Documents/MasqueRouge/masquerouge/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{711D3FBF-07CF-0D49-B9A3-A6681EA5390F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E6C5E1-AB5D-6344-8E09-E33049928652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{62FA4379-BE8B-AB47-BACB-4FB9744D6952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>SP Restantes</t>
   </si>
@@ -141,6 +141,9 @@
       </rPr>
       <t>December 16th</t>
     </r>
+  </si>
+  <si>
+    <t>Sprints Restantes</t>
   </si>
 </sst>
 </file>
@@ -364,20 +367,8 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -393,7 +384,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,6 +406,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81F22E7-80B8-5043-9822-B8998C10B3D5}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,13 +745,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -756,264 +759,264 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="15">
         <f>71</f>
         <v>71</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="21"/>
+      <c r="G3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="B5" s="11">
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13">
-        <v>3</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8">
-        <v>21</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="8">
-        <v>8</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8">
-        <v>3</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="7">
         <f>SUM(H5:H6)</f>
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>8</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>5</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>8</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>5</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="7">
         <f>SUM(E5:E14)</f>
         <v>71</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="7">
         <f>SUM(H12:H15)</f>
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="4:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="4:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="4:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="7">
         <f>SUM(H20:H23)</f>
         <v>23</v>
       </c>

</xml_diff>